<commit_message>
Imbalanced testing done on all three IEEE systems
</commit_message>
<xml_diff>
--- a/Plots and Figures/Raw_Results/RESULTS_IEEE14_MainModelsTest_earlyStop_100Epochs.xlsx
+++ b/Plots and Figures/Raw_Results/RESULTS_IEEE14_MainModelsTest_earlyStop_100Epochs.xlsx
@@ -456,13 +456,13 @@
         <v>0.7394999861717224</v>
       </c>
       <c r="D2">
-        <v>0.8859999775886536</v>
+        <v>0.9070000052452087</v>
       </c>
       <c r="E2">
         <v>0.647734956051386</v>
       </c>
       <c r="F2">
-        <v>0.871331828442438</v>
+        <v>0.8974641675854464</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -474,7 +474,7 @@
         <v>0.479</v>
       </c>
       <c r="J2">
-        <v>0.772</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -494,13 +494,13 @@
         <v>0.8324999809265137</v>
       </c>
       <c r="D3">
-        <v>0.953499972820282</v>
+        <v>0.9605000019073486</v>
       </c>
       <c r="E3">
         <v>0.7987987987987988</v>
       </c>
       <c r="F3">
-        <v>0.951232302045097</v>
+        <v>0.9588755856324831</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -512,7 +512,7 @@
         <v>0.665</v>
       </c>
       <c r="J3">
-        <v>0.907</v>
+        <v>0.921</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -532,13 +532,13 @@
         <v>0.8840000033378601</v>
       </c>
       <c r="D4">
-        <v>0.9720000028610229</v>
+        <v>0.9800000190734863</v>
       </c>
       <c r="E4">
         <v>0.8687782805429864</v>
       </c>
       <c r="F4">
-        <v>0.9711934156378601</v>
+        <v>0.9795918367346939</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -550,7 +550,7 @@
         <v>0.768</v>
       </c>
       <c r="J4">
-        <v>0.944</v>
+        <v>0.96</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -570,13 +570,13 @@
         <v>0.9169999957084656</v>
       </c>
       <c r="D5">
-        <v>0.9829999804496765</v>
+        <v>0.9890000224113464</v>
       </c>
       <c r="E5">
         <v>0.9094874591057797</v>
       </c>
       <c r="F5">
-        <v>0.982706002034588</v>
+        <v>0.9888776541961577</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -588,7 +588,7 @@
         <v>0.834</v>
       </c>
       <c r="J5">
-        <v>0.966</v>
+        <v>0.978</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -608,31 +608,31 @@
         <v>0.9265000224113464</v>
       </c>
       <c r="D6">
-        <v>0.9950000047683716</v>
+        <v>0.996999979019165</v>
       </c>
       <c r="E6">
         <v>0.9207547169811321</v>
       </c>
       <c r="F6">
-        <v>0.9949748743718593</v>
+        <v>0.9969939879759518</v>
       </c>
       <c r="G6">
         <v>0.9988304093567252</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0.998995983935743</v>
       </c>
       <c r="I6">
         <v>0.854</v>
       </c>
       <c r="J6">
-        <v>0.99</v>
+        <v>0.995</v>
       </c>
       <c r="K6">
         <v>0.001</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -646,13 +646,13 @@
         <v>0.8995000123977661</v>
       </c>
       <c r="D7">
-        <v>0.987500011920929</v>
+        <v>0.9909999966621399</v>
       </c>
       <c r="E7">
         <v>0.8882712618121179</v>
       </c>
       <c r="F7">
-        <v>0.9873417721518987</v>
+        <v>0.9909182643794148</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -664,7 +664,7 @@
         <v>0.799</v>
       </c>
       <c r="J7">
-        <v>0.975</v>
+        <v>0.982</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -684,13 +684,13 @@
         <v>0.8859999775886536</v>
       </c>
       <c r="D8">
-        <v>0.9894999861717224</v>
+        <v>0.9934999942779541</v>
       </c>
       <c r="E8">
         <v>0.871331828442438</v>
       </c>
       <c r="F8">
-        <v>0.989388580090955</v>
+        <v>0.9934574735782586</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -702,7 +702,7 @@
         <v>0.772</v>
       </c>
       <c r="J8">
-        <v>0.979</v>
+        <v>0.987</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -722,19 +722,19 @@
         <v>0.9879999756813049</v>
       </c>
       <c r="D9">
-        <v>0.9994999766349792</v>
+        <v>0.9990000128746033</v>
       </c>
       <c r="E9">
         <v>0.9878542510121457</v>
       </c>
       <c r="F9">
-        <v>0.9995002498750626</v>
+        <v>0.9990009990009989</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.999000999000999</v>
+        <v>0.998003992015968</v>
       </c>
       <c r="I9">
         <v>0.976</v>
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -760,13 +760,13 @@
         <v>0.9769999980926514</v>
       </c>
       <c r="D10">
-        <v>0.9980000257492065</v>
+        <v>0.9990000128746033</v>
       </c>
       <c r="E10">
         <v>0.9764585465711361</v>
       </c>
       <c r="F10">
-        <v>0.9979959919839679</v>
+        <v>0.998998998998999</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -778,7 +778,7 @@
         <v>0.954</v>
       </c>
       <c r="J10">
-        <v>0.996</v>
+        <v>0.998</v>
       </c>
       <c r="K10">
         <v>0</v>

</xml_diff>